<commit_message>
Thêm file Excel kết quả Ma_so_thue_doanh_nghiep.xlsx
</commit_message>
<xml_diff>
--- a/Ma_so_thue_doanh_nghiep.xlsx
+++ b/Ma_so_thue_doanh_nghiep.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Trang_1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Trang_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Trang_3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Trang_4" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +428,25 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,12 +474,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5200951139</t>
+          <t>3604022682</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CÔNG TY TNHH TM VÀ DV NÔNG NGHIỆP KIÊN PHONG</t>
+          <t>CÔNG TY TNHH N.S AUTO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -470,12 +491,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0318992469</t>
+          <t>0318993448</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CÔNG TY TNHH DƯỢC KCP</t>
+          <t>CÔNG TY TNHH TMDV VT XD QUỐC PHƯƠNG</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -487,12 +508,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5000906361</t>
+          <t>0801451533</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CÔNG TY TNHH THƯƠNG MẠI M&amp;M</t>
+          <t>CÔNG TY TNHH XÂY DỰNG VÀ VẬN TẢI BẢO LINH</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -504,12 +525,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1501155704</t>
+          <t>0111082350</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CÔNG TY TNHH SƠN - NGỌC DANH</t>
+          <t>CÔNG TY TNHH THƯƠNG MẠI VÀ DỊCH VỤ LOAN TÙNG</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -521,12 +542,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0111079679</t>
+          <t>1702317842</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CÔNG TY CỔ PHẦN TẬP ĐOÀN AINOVA VIỆT NAM</t>
+          <t>CÔNG TY TNHH THƯƠNG MẠI - DỊCH VỤ DU LỊCH THỚI AN KHÁNH AN</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -538,15 +559,1821 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>0318992483</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ĐẦU TƯ KINH DOANH BẤT ĐỘNG SẢN 186</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0318990398</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THỰC PHẨM BÒ VUI</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0315295438</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ROBOCASH VIỆT NAM (NT)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>09/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2301337674</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH CÔNG NGHỆ YUESHENGXIN</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0111082329</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH XÂY DỰNG BẰNG TUYẾT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0318987652</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH NET 269 TRƯƠNG THỊ HOA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>5200951139</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TM VÀ DV NÔNG NGHIỆP KIÊN PHONG</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0318992469</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH DƯỢC KCP</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5000906361</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI M&amp;M</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1501155704</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH SƠN - NGỌC DANH</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>0111079679</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN TẬP ĐOÀN AINOVA VIỆT NAM</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>3002291511</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TM &amp; DV KHẢ NHƯ GROUP</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1801791725</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH SẢN XUẤT INOX TMDV XUÂN AN PHÚC</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0318992236</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI GAS TRƯỜNG THỊNH</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>1602198408</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH VLXD MINH NHỰT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>3002291455</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TRUNG LINH CT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0601287036</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH DỊCH VỤ THƯƠNG MẠI VÀ XUẤT NHẬP KHẨU THIÊN TRƯỜNG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>5702186964</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH HOA NAM ĐÔNG MAI</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Mã số thuế</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Tên doanh nghiệp</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ngày cấp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>3604022682</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH N.S AUTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0318993448</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TMDV VT XD QUỐC PHƯƠNG</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0801451533</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH XÂY DỰNG VÀ VẬN TẢI BẢO LINH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0111082350</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI VÀ DỊCH VỤ LOAN TÙNG</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1702317842</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI - DỊCH VỤ DU LỊCH THỚI AN KHÁNH AN</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>0318992483</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>CÔNG TY TNHH ĐẦU TƯ KINH DOANH BẤT ĐỘNG SẢN 186</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0318990398</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THỰC PHẨM BÒ VUI</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0315295438</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ROBOCASH VIỆT NAM (NT)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>09/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2301337674</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH CÔNG NGHỆ YUESHENGXIN</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0111082329</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH XÂY DỰNG BẰNG TUYẾT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0318987652</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH NET 269 TRƯƠNG THỊ HOA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>5200951139</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TM VÀ DV NÔNG NGHIỆP KIÊN PHONG</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0318992469</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH DƯỢC KCP</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5000906361</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI M&amp;M</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1501155704</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH SƠN - NGỌC DANH</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>0111079679</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN TẬP ĐOÀN AINOVA VIỆT NAM</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>3002291511</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>CÔNG TY TNHH TM &amp; DV KHẢ NHƯ GROUP</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1801791725</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH SẢN XUẤT INOX TMDV XUÂN AN PHÚC</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0318992236</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI GAS TRƯỜNG THỊNH</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>1602198408</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH VLXD MINH NHỰT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>3002291455</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TRUNG LINH CT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0601287036</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH DỊCH VỤ THƯƠNG MẠI VÀ XUẤT NHẬP KHẨU THIÊN TRƯỜNG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>5702186964</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH HOA NAM ĐÔNG MAI</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>4101658836</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH GIÁO DỤC ÁNH DƯƠNG QUY NHƠN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2301337681</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH VICO NLTP</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>6200127237</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH MTV XÂY DỰNG THƯƠNG MẠI ĐỨC CẢNH</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2301337498</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ĐÀO TẠO NGHỆ THUẬT THỂ THAO ÁNH DƯƠNG</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>3604023083</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI DỊCH VỤ SANG PHÚ</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>5702186763</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ĐẦU TƯ VÀ THƯƠNG MẠI DỊCH VỤ TIẾN DŨNG</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2902227732</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI VÀ DỊCH VỤ XUÂN MÙI</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0901192071</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TM &amp; DV A-Z VINA HƯNG YÊN</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>1102100076</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN TM DV DYV</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2700979715</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN THANH LONG BIOMASS NB</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>0111079975</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI TỊNH LUYẾN</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>0318992490</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI KỸ THUẬT PHAN HẢI</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Mã số thuế</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Tên doanh nghiệp</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ngày cấp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>3604022682</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH N.S AUTO</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>0318993448</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TMDV VT XD QUỐC PHƯƠNG</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0801451533</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH XÂY DỰNG VÀ VẬN TẢI BẢO LINH</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>0111082350</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI VÀ DỊCH VỤ LOAN TÙNG</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1702317842</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI - DỊCH VỤ DU LỊCH THỚI AN KHÁNH AN</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>0318992483</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ĐẦU TƯ KINH DOANH BẤT ĐỘNG SẢN 186</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>0318990398</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THỰC PHẨM BÒ VUI</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>0315295438</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ROBOCASH VIỆT NAM (NT)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>09/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2301337674</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH CÔNG NGHỆ YUESHENGXIN</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>0111082329</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH XÂY DỰNG BẰNG TUYẾT</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>0318987652</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH NET 269 TRƯƠNG THỊ HOA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>5200951139</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TM VÀ DV NÔNG NGHIỆP KIÊN PHONG</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>0318992469</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH DƯỢC KCP</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>5000906361</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI M&amp;M</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1501155704</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH SƠN - NGỌC DANH</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>0111079679</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN TẬP ĐOÀN AINOVA VIỆT NAM</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>3002291511</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TM &amp; DV KHẢ NHƯ GROUP</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1801791725</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH SẢN XUẤT INOX TMDV XUÂN AN PHÚC</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0318992236</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI GAS TRƯỜNG THỊNH</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>1602198408</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH VLXD MINH NHỰT</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>3002291455</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TRUNG LINH CT</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0601287036</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH DỊCH VỤ THƯƠNG MẠI VÀ XUẤT NHẬP KHẨU THIÊN TRƯỜNG</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>5702186964</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH HOA NAM ĐÔNG MAI</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>4101658836</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH GIÁO DỤC ÁNH DƯƠNG QUY NHƠN</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2301337681</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH VICO NLTP</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>6200127237</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH MTV XÂY DỰNG THƯƠNG MẠI ĐỨC CẢNH</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2301337498</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ĐÀO TẠO NGHỆ THUẬT THỂ THAO ÁNH DƯƠNG</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>3604023083</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI DỊCH VỤ SANG PHÚ</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>5702186763</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH ĐẦU TƯ VÀ THƯƠNG MẠI DỊCH VỤ TIẾN DŨNG</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2902227732</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI VÀ DỊCH VỤ XUÂN MÙI</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0901192071</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TM &amp; DV A-Z VINA HƯNG YÊN</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>1102100076</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN TM DV DYV</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2700979715</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN THANH LONG BIOMASS NB</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>0111079975</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI TỊNH LUYẾN</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>0318992490</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI KỸ THUẬT PHAN HẢI</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>3604022805</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THƯƠNG MẠI DỊCH VỤ LINH TRÂN</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>3502548204</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH VẬN TẢI LOGISTICS GIA HÂN</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>4900870268</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN TRUYỀN THÔNG CÔNG NGHỆ SỐ PHƯƠNG ĐÔNG</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>10/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>0318992148</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH NĂNG LƯỢNG PHÚ SĨ</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>5901224082</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH MTV HOÀI NAM GIA LAI</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>0601287131</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH VẬN TẢI VÀ THƯƠNG MẠI VLXD TUẤN KHOÁI</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>5801537250</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TM DV TÙNG HIỀN</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>0318991881</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH PHI'S</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>0318992194</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH THIẾT KẾ XÂY DỰNG NHÀ ĐẸP DK</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>0318993423</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH NHANG TÂN VẬN LỢI</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>0105924224-001</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>CHI NHÁNH PHÚ QUỐC - CÔNG TY TNHH BẤT ĐỘNG SẢN NEWVISION</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>09/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>1801791612</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH TERRA MEDIA</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>3002291529</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH MỘT TV BẢO HƯNG</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>06/2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>0105924224</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH BẤT ĐỘNG SẢN NEWVISION</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>06/2012</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>1801791718</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>CÔNG TY TNHH XÂY DỰNG VÀ THƯƠNG MẠI HUY HOÀNG CN</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
         <is>
           <t>06/2025</t>
         </is>

</xml_diff>